<commit_message>
Add data used for Simulation - 6 months
</commit_message>
<xml_diff>
--- a/document/Simulation.xlsx
+++ b/document/Simulation.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="4545" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="4545" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Solver" sheetId="1" r:id="rId1"/>
     <sheet name="Time" sheetId="2" r:id="rId2"/>
     <sheet name="New Cost" sheetId="3" r:id="rId3"/>
+    <sheet name="Data" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="93">
   <si>
     <t>Utility</t>
   </si>
@@ -122,6 +123,189 @@
   </si>
   <si>
     <t>gap</t>
+  </si>
+  <si>
+    <t>Quarterly</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Location x</t>
+  </si>
+  <si>
+    <t>Location y</t>
+  </si>
+  <si>
+    <t>numApts</t>
+  </si>
+  <si>
+    <t>2017-Q3</t>
+  </si>
+  <si>
+    <t>Sky Vista</t>
+  </si>
+  <si>
+    <t>West Scape</t>
+  </si>
+  <si>
+    <t>Rivervale Shores</t>
+  </si>
+  <si>
+    <t>2017-Q2</t>
+  </si>
+  <si>
+    <t>Marsiling Grove</t>
+  </si>
+  <si>
+    <t>103.77.4341</t>
+  </si>
+  <si>
+    <t>Woodlands Spring</t>
+  </si>
+  <si>
+    <t>Forest Spring</t>
+  </si>
+  <si>
+    <t>Woodleigh Hillside</t>
+  </si>
+  <si>
+    <t>Dakota Breeze</t>
+  </si>
+  <si>
+    <t>Pine Vista</t>
+  </si>
+  <si>
+    <t>2017-Q1</t>
+  </si>
+  <si>
+    <t>Northshore Cove</t>
+  </si>
+  <si>
+    <t>Waterway Sunrise II</t>
+  </si>
+  <si>
+    <t>Clementi NorthArc</t>
+  </si>
+  <si>
+    <t>Clementi Peaks</t>
+  </si>
+  <si>
+    <t>Tampines GreenBloom</t>
+  </si>
+  <si>
+    <t>Tampines GreenFlora</t>
+  </si>
+  <si>
+    <t>2016-Q4</t>
+  </si>
+  <si>
+    <t>Matilda Sundeck</t>
+  </si>
+  <si>
+    <t>Northshore Trio</t>
+  </si>
+  <si>
+    <t>Waterway Sunrise I</t>
+  </si>
+  <si>
+    <t>Bedok Beacon</t>
+  </si>
+  <si>
+    <t>Bedok North Vale</t>
+  </si>
+  <si>
+    <t>Bedok South Horizon</t>
+  </si>
+  <si>
+    <t>Woodleigh Glen</t>
+  </si>
+  <si>
+    <t>Woodleigh Village</t>
+  </si>
+  <si>
+    <t>Kalang Residences</t>
+  </si>
+  <si>
+    <t>2016-Q3</t>
+  </si>
+  <si>
+    <t>Buangkok Woods</t>
+  </si>
+  <si>
+    <t>EastDelta @Canberra</t>
+  </si>
+  <si>
+    <t>Valley Spring</t>
+  </si>
+  <si>
+    <t>Tampines GreenView</t>
+  </si>
+  <si>
+    <t>Tampines GreenVerge</t>
+  </si>
+  <si>
+    <t>2016-Q2</t>
+  </si>
+  <si>
+    <t>EastCreek @Canberra</t>
+  </si>
+  <si>
+    <t>Senja Valley</t>
+  </si>
+  <si>
+    <t>Senja Heights</t>
+  </si>
+  <si>
+    <t>Senja Ridges</t>
+  </si>
+  <si>
+    <t>Ang Mo Kio Court</t>
+  </si>
+  <si>
+    <t>Bedok North Woods</t>
+  </si>
+  <si>
+    <t>2016-Q1</t>
+  </si>
+  <si>
+    <t>West Plains</t>
+  </si>
+  <si>
+    <t>Anchorvale Plains</t>
+  </si>
+  <si>
+    <t>Alkaff Oasis</t>
+  </si>
+  <si>
+    <t>2015-Q4</t>
+  </si>
+  <si>
+    <t>Teck Whye Vista</t>
+  </si>
+  <si>
+    <t>Fernvale Woods</t>
+  </si>
+  <si>
+    <t>West Quarry</t>
+  </si>
+  <si>
+    <t>Hougang RiverCourt</t>
+  </si>
+  <si>
+    <t>Waterfront I &amp; II @Northshore</t>
+  </si>
+  <si>
+    <t>Northshore StraitsView</t>
+  </si>
+  <si>
+    <t>Alkaff CourtView</t>
+  </si>
+  <si>
+    <t>Alkaff LakeView</t>
+  </si>
+  <si>
+    <t>Alkaff Vista</t>
   </si>
 </sst>
 </file>
@@ -151,7 +335,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -196,11 +380,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -211,11 +425,194 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -279,6 +676,20 @@
     <tableColumn id="8" name="min"/>
     <tableColumn id="9" name="max"/>
     <tableColumn id="10" name="gap"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:E48" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="A1:E48"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Quarterly" dataDxfId="4"/>
+    <tableColumn id="2" name="Project" dataDxfId="3"/>
+    <tableColumn id="3" name="Location x" dataDxfId="2"/>
+    <tableColumn id="4" name="Location y" dataDxfId="1"/>
+    <tableColumn id="5" name="numApts"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1513,7 +1924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+    <sheetView topLeftCell="A68" workbookViewId="0">
       <selection activeCell="E96" sqref="E96:J96"/>
     </sheetView>
   </sheetViews>
@@ -4575,4 +4986,730 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="10">
+        <v>103.745318</v>
+      </c>
+      <c r="D2" s="10">
+        <v>1.35022</v>
+      </c>
+      <c r="E2" s="6">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="11">
+        <v>103.74143100000001</v>
+      </c>
+      <c r="D3" s="11">
+        <v>1.3621209999999999</v>
+      </c>
+      <c r="E3">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="10">
+        <v>103.91282</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1.3874759999999999</v>
+      </c>
+      <c r="E4">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="11">
+        <v>1.4374709999999999</v>
+      </c>
+      <c r="E5">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="10">
+        <v>103.799753</v>
+      </c>
+      <c r="D6" s="10">
+        <v>1.446501</v>
+      </c>
+      <c r="E6">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="11">
+        <v>103.85252300000001</v>
+      </c>
+      <c r="D7" s="11">
+        <v>1.4258439999999999</v>
+      </c>
+      <c r="E7">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="10">
+        <v>103.874274</v>
+      </c>
+      <c r="D8" s="10">
+        <v>1.3423609999999999</v>
+      </c>
+      <c r="E8">
+        <v>1355</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="11">
+        <v>103.888105</v>
+      </c>
+      <c r="D9" s="11">
+        <v>1.309895</v>
+      </c>
+      <c r="E9">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="10">
+        <v>103.885718</v>
+      </c>
+      <c r="D10" s="10">
+        <v>1.3096479999999999</v>
+      </c>
+      <c r="E10">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="11">
+        <v>103.906594</v>
+      </c>
+      <c r="D11" s="11">
+        <v>1.419826</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="10">
+        <v>103.920834</v>
+      </c>
+      <c r="D12" s="10">
+        <v>1.397653</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="11">
+        <v>103.76343199999999</v>
+      </c>
+      <c r="D13" s="11">
+        <v>1.3224959999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="10">
+        <v>103.767605</v>
+      </c>
+      <c r="D14" s="10">
+        <v>1.310033</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="11">
+        <v>103.930182</v>
+      </c>
+      <c r="D15" s="11">
+        <v>1.353442</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="10">
+        <v>103.930632</v>
+      </c>
+      <c r="D16" s="10">
+        <v>1.3541179999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="11">
+        <v>103.893292</v>
+      </c>
+      <c r="D17" s="11">
+        <v>1.4030560000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="10">
+        <v>103.905901</v>
+      </c>
+      <c r="D18" s="10">
+        <v>1.417945</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="11">
+        <v>103.921026</v>
+      </c>
+      <c r="D19" s="11">
+        <v>1.3989279999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="10">
+        <v>103.927797</v>
+      </c>
+      <c r="D20" s="10">
+        <v>1.324578</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="11">
+        <v>103.92563800000001</v>
+      </c>
+      <c r="D21" s="11">
+        <v>1.329966</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="10">
+        <v>103.947209</v>
+      </c>
+      <c r="D22" s="10">
+        <v>1.3179160000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="11">
+        <v>103.87165400000001</v>
+      </c>
+      <c r="D23" s="11">
+        <v>1.341952</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="10">
+        <v>103.87164300000001</v>
+      </c>
+      <c r="D24" s="10">
+        <v>1.3406439999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="11">
+        <v>103.872784</v>
+      </c>
+      <c r="D25" s="11">
+        <v>1.3116570000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="10">
+        <v>103.881237</v>
+      </c>
+      <c r="D26" s="10">
+        <v>1.38107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="11">
+        <v>103.835064</v>
+      </c>
+      <c r="D27" s="11">
+        <v>1.445864</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="10">
+        <v>103.85086200000001</v>
+      </c>
+      <c r="D28" s="10">
+        <v>1.4293039999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="11">
+        <v>103.935441</v>
+      </c>
+      <c r="D29" s="11">
+        <v>1.3657349999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="10">
+        <v>103.94006899999999</v>
+      </c>
+      <c r="D30" s="10">
+        <v>1.3617319999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" s="11">
+        <v>103.831208</v>
+      </c>
+      <c r="D31" s="11">
+        <v>1.4514020000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" s="10">
+        <v>103.763017</v>
+      </c>
+      <c r="D32" s="10">
+        <v>1.38767</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="11">
+        <v>103.76218799999999</v>
+      </c>
+      <c r="D33" s="11">
+        <v>1.3873260000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="10">
+        <v>103.761563</v>
+      </c>
+      <c r="D34" s="10">
+        <v>1.3886780000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" s="11">
+        <v>103.840058</v>
+      </c>
+      <c r="D35" s="11">
+        <v>1.3678920000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="10">
+        <v>103.93249299999999</v>
+      </c>
+      <c r="D36" s="10">
+        <v>1.330408</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="11">
+        <v>103.742814</v>
+      </c>
+      <c r="D37" s="11">
+        <v>1.356976</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="10">
+        <v>103.885017</v>
+      </c>
+      <c r="D38" s="10">
+        <v>1.393551</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" s="11">
+        <v>103.87262800000001</v>
+      </c>
+      <c r="D39" s="11">
+        <v>1.334657</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" s="10">
+        <v>103.75862100000001</v>
+      </c>
+      <c r="D40" s="10">
+        <v>1.379089</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="11">
+        <v>103.870385</v>
+      </c>
+      <c r="D41" s="11">
+        <v>1.3921289999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="10">
+        <v>103.739622</v>
+      </c>
+      <c r="D42" s="10">
+        <v>1.353844</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" s="11">
+        <v>103.894946</v>
+      </c>
+      <c r="D43" s="11">
+        <v>1.362646</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="10">
+        <v>103.901758</v>
+      </c>
+      <c r="D44" s="10">
+        <v>1.4177599999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="11">
+        <v>103.904578</v>
+      </c>
+      <c r="D45" s="11">
+        <v>1.419303</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="10">
+        <v>103.871205</v>
+      </c>
+      <c r="D46" s="10">
+        <v>1.336476</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47" s="11">
+        <v>103.872535</v>
+      </c>
+      <c r="D47" s="11">
+        <v>1.336905</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48" s="12">
+        <v>103.87011699999999</v>
+      </c>
+      <c r="D48" s="12">
+        <v>1.3334490000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>